<commit_message>
feat: add struct to excel
</commit_message>
<xml_diff>
--- a/test_excel_file/test_write.xlsx
+++ b/test_excel_file/test_write.xlsx
@@ -7,7 +7,6 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Infos" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -352,22 +351,11 @@
 </theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -386,35 +374,49 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix:zero value set err
</commit_message>
<xml_diff>
--- a/test_excel_file/test_write.xlsx
+++ b/test_excel_file/test_write.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>user_name</t>
   </si>
@@ -28,6 +28,15 @@
     <t>man</t>
   </si>
   <si>
+    <t>person name</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>booyang</t>
   </si>
   <si>
@@ -44,9 +53,6 @@
   </si>
   <si>
     <t>14</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>shanghai</t>
@@ -374,50 +380,50 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>